<commit_message>
Add requirements and improve .gitignore
</commit_message>
<xml_diff>
--- a/processed_excel.xlsx
+++ b/processed_excel.xlsx
@@ -16,19 +16,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
-    <t>Indice</t>
+    <t>Index</t>
   </si>
   <si>
     <t>Id</t>
   </si>
   <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Profesion</t>
-  </si>
-  <si>
-    <t>Sueldo</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Profession</t>
+  </si>
+  <si>
+    <t>Salary</t>
   </si>
   <si>
     <t>Total</t>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">     Juan Perez     </t>
   </si>
   <si>
-    <t xml:space="preserve">     INGENIERO      </t>
+    <t xml:space="preserve">      ENGINNER      </t>
   </si>
   <si>
     <t xml:space="preserve">        200         </t>
@@ -61,7 +61,7 @@
     <t xml:space="preserve">     Ana Lopez      </t>
   </si>
   <si>
-    <t xml:space="preserve">      CONTADOR      </t>
+    <t xml:space="preserve">      COUNTER       </t>
   </si>
   <si>
     <t xml:space="preserve">        180         </t>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">    Dario Ojeda     </t>
   </si>
   <si>
-    <t xml:space="preserve">       MEDICO       </t>
+    <t xml:space="preserve">       DOCTOR       </t>
   </si>
   <si>
     <t xml:space="preserve">        350         </t>
@@ -97,7 +97,7 @@
     <t xml:space="preserve">    Rosa Fuentes    </t>
   </si>
   <si>
-    <t xml:space="preserve">     PSICOLOGA      </t>
+    <t xml:space="preserve">    PSYCHOLOGIST    </t>
   </si>
   <si>
     <t xml:space="preserve">        190         </t>
@@ -115,7 +115,7 @@
     <t xml:space="preserve">   Domingo Masias   </t>
   </si>
   <si>
-    <t xml:space="preserve">    PROGRAMADOR     </t>
+    <t xml:space="preserve">     PROGRAMMER     </t>
   </si>
   <si>
     <t xml:space="preserve">        250         </t>
@@ -500,8 +500,8 @@
   <cols>
     <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="17.719285714285714" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>

</xml_diff>